<commit_message>
20T to 21T map update data element group
</commit_message>
<xml_diff>
--- a/data-raw/snu_x_im_distribution_configuration/20Tto21TMap.xlsx
+++ b/data-raw/snu_x_im_distribution_configuration/20Tto21TMap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/snu_x_im_distribution_configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{DD78BCF7-51E1-3D48-8822-722F8EEB1BB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{DF270AA2-15E0-3E47-B4E3-CC419906039A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="460" windowWidth="25600" windowHeight="20020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1113,9 +1113,6 @@
     <t>pe</t>
   </si>
   <si>
-    <t>DE_GROUP-zhdJiWlPvCz</t>
-  </si>
-  <si>
     <t>2018Oct</t>
   </si>
   <si>
@@ -1351,6 +1348,9 @@
   </si>
   <si>
     <t>indicatorCode_fy20_cop</t>
+  </si>
+  <si>
+    <t>DE_GROUP-XUA8pDYjPsw</t>
   </si>
 </sst>
 </file>
@@ -2224,8 +2224,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2235,7 +2235,7 @@
     <col min="3" max="3" width="31.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.83203125" bestFit="1" customWidth="1"/>
@@ -2252,7 +2252,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>298</v>
@@ -2308,7 +2308,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>10</v>
@@ -2323,7 +2323,7 @@
         <v>12</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>10</v>
@@ -2344,7 +2344,7 @@
         <v>355</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>9</v>
@@ -2364,7 +2364,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>10</v>
@@ -2379,7 +2379,7 @@
         <v>13</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>10</v>
@@ -2400,7 +2400,7 @@
         <v>355</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N3" s="4" t="s">
         <v>9</v>
@@ -2420,7 +2420,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>14</v>
@@ -2435,7 +2435,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>42</v>
@@ -2456,7 +2456,7 @@
         <v>339</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>137</v>
@@ -2476,7 +2476,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>14</v>
@@ -2491,7 +2491,7 @@
         <v>17</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>42</v>
@@ -2512,7 +2512,7 @@
         <v>339</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N5" s="4" t="s">
         <v>137</v>
@@ -2532,7 +2532,7 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>18</v>
@@ -2547,7 +2547,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>42</v>
@@ -2568,7 +2568,7 @@
         <v>338</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N6" s="4" t="s">
         <v>137</v>
@@ -2588,7 +2588,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>18</v>
@@ -2603,7 +2603,7 @@
         <v>17</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>42</v>
@@ -2624,7 +2624,7 @@
         <v>338</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N7" s="4" t="s">
         <v>137</v>
@@ -2644,7 +2644,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>24</v>
@@ -2659,7 +2659,7 @@
         <v>26</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>24</v>
@@ -2680,7 +2680,7 @@
         <v>334</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N8" s="4" t="s">
         <v>135</v>
@@ -2700,7 +2700,7 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>24</v>
@@ -2715,7 +2715,7 @@
         <v>28</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>24</v>
@@ -2736,7 +2736,7 @@
         <v>334</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N9" s="4" t="s">
         <v>135</v>
@@ -2756,7 +2756,7 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>29</v>
@@ -2771,7 +2771,7 @@
         <v>30</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>42</v>
@@ -2792,7 +2792,7 @@
         <v>337</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N10" s="4" t="s">
         <v>137</v>
@@ -2812,7 +2812,7 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>29</v>
@@ -2827,7 +2827,7 @@
         <v>31</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>42</v>
@@ -2848,7 +2848,7 @@
         <v>337</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N11" s="4" t="s">
         <v>137</v>
@@ -2868,7 +2868,7 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>32</v>
@@ -2883,7 +2883,7 @@
         <v>30</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>42</v>
@@ -2904,7 +2904,7 @@
         <v>340</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N12" s="4" t="s">
         <v>137</v>
@@ -2924,7 +2924,7 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>32</v>
@@ -2939,7 +2939,7 @@
         <v>31</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>42</v>
@@ -2960,7 +2960,7 @@
         <v>340</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N13" s="4" t="s">
         <v>137</v>
@@ -2980,7 +2980,7 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>33</v>
@@ -2995,7 +2995,7 @@
         <v>30</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>42</v>
@@ -3016,7 +3016,7 @@
         <v>344</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N14" s="4" t="s">
         <v>139</v>
@@ -3036,7 +3036,7 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>33</v>
@@ -3051,7 +3051,7 @@
         <v>31</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>42</v>
@@ -3072,7 +3072,7 @@
         <v>344</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N15" s="4" t="s">
         <v>139</v>
@@ -3092,7 +3092,7 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>34</v>
@@ -3107,7 +3107,7 @@
         <v>30</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>42</v>
@@ -3128,7 +3128,7 @@
         <v>356</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N16" s="4" t="s">
         <v>137</v>
@@ -3148,7 +3148,7 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>34</v>
@@ -3163,7 +3163,7 @@
         <v>31</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>42</v>
@@ -3184,7 +3184,7 @@
         <v>356</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N17" s="4" t="s">
         <v>137</v>
@@ -3204,7 +3204,7 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>35</v>
@@ -3219,7 +3219,7 @@
         <v>30</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>42</v>
@@ -3240,7 +3240,7 @@
         <v>347</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N18" s="4" t="s">
         <v>137</v>
@@ -3260,7 +3260,7 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>35</v>
@@ -3275,7 +3275,7 @@
         <v>31</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>42</v>
@@ -3296,7 +3296,7 @@
         <v>347</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N19" s="4" t="s">
         <v>137</v>
@@ -3316,7 +3316,7 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>36</v>
@@ -3331,7 +3331,7 @@
         <v>30</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>42</v>
@@ -3352,7 +3352,7 @@
         <v>348</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N20" s="4" t="s">
         <v>137</v>
@@ -3372,7 +3372,7 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>36</v>
@@ -3387,7 +3387,7 @@
         <v>31</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>42</v>
@@ -3408,7 +3408,7 @@
         <v>348</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N21" s="4" t="s">
         <v>137</v>
@@ -3428,7 +3428,7 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>37</v>
@@ -3443,7 +3443,7 @@
         <v>30</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>42</v>
@@ -3464,7 +3464,7 @@
         <v>349</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N22" s="4" t="s">
         <v>139</v>
@@ -3484,7 +3484,7 @@
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>37</v>
@@ -3499,7 +3499,7 @@
         <v>31</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>42</v>
@@ -3520,7 +3520,7 @@
         <v>349</v>
       </c>
       <c r="M23" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N23" s="4" t="s">
         <v>139</v>
@@ -3540,7 +3540,7 @@
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>38</v>
@@ -3555,7 +3555,7 @@
         <v>30</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>42</v>
@@ -3576,7 +3576,7 @@
         <v>350</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N24" s="4" t="s">
         <v>137</v>
@@ -3596,7 +3596,7 @@
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>38</v>
@@ -3611,7 +3611,7 @@
         <v>31</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>42</v>
@@ -3632,7 +3632,7 @@
         <v>350</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N25" s="4" t="s">
         <v>137</v>
@@ -3652,7 +3652,7 @@
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>39</v>
@@ -3667,7 +3667,7 @@
         <v>30</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>42</v>
@@ -3688,7 +3688,7 @@
         <v>352</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N26" s="4" t="s">
         <v>137</v>
@@ -3708,7 +3708,7 @@
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>39</v>
@@ -3723,7 +3723,7 @@
         <v>31</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>42</v>
@@ -3744,7 +3744,7 @@
         <v>352</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N27" s="4" t="s">
         <v>137</v>
@@ -3764,7 +3764,7 @@
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>40</v>
@@ -3779,7 +3779,7 @@
         <v>30</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>42</v>
@@ -3800,7 +3800,7 @@
         <v>353</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N28" s="4" t="s">
         <v>137</v>
@@ -3820,7 +3820,7 @@
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>40</v>
@@ -3835,7 +3835,7 @@
         <v>31</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>42</v>
@@ -3856,7 +3856,7 @@
         <v>353</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N29" s="4" t="s">
         <v>137</v>
@@ -3876,7 +3876,7 @@
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>41</v>
@@ -3891,7 +3891,7 @@
         <v>30</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>42</v>
@@ -3912,7 +3912,7 @@
         <v>354</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N30" s="4" t="s">
         <v>137</v>
@@ -3932,7 +3932,7 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>41</v>
@@ -3947,7 +3947,7 @@
         <v>31</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>42</v>
@@ -3968,7 +3968,7 @@
         <v>354</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N31" s="4" t="s">
         <v>137</v>
@@ -3988,7 +3988,7 @@
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>42</v>
@@ -4003,7 +4003,7 @@
         <v>30</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>42</v>
@@ -4024,7 +4024,7 @@
         <v>343</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N32" s="4" t="s">
         <v>9</v>
@@ -4044,7 +4044,7 @@
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>42</v>
@@ -4059,7 +4059,7 @@
         <v>31</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>42</v>
@@ -4080,7 +4080,7 @@
         <v>343</v>
       </c>
       <c r="M33" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N33" s="4" t="s">
         <v>9</v>
@@ -4100,7 +4100,7 @@
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>44</v>
@@ -4115,7 +4115,7 @@
         <v>9</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>44</v>
@@ -4136,7 +4136,7 @@
         <v>351</v>
       </c>
       <c r="M34" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N34" s="4" t="s">
         <v>9</v>
@@ -4156,7 +4156,7 @@
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>46</v>
@@ -4171,7 +4171,7 @@
         <v>9</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>46</v>
@@ -4192,7 +4192,7 @@
         <v>341</v>
       </c>
       <c r="M35" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N35" s="4" t="s">
         <v>9</v>
@@ -4212,7 +4212,7 @@
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>48</v>
@@ -4227,7 +4227,7 @@
         <v>9</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G36" s="4" t="s">
         <v>48</v>
@@ -4248,7 +4248,7 @@
         <v>346</v>
       </c>
       <c r="M36" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N36" s="4" t="s">
         <v>9</v>
@@ -4268,7 +4268,7 @@
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>50</v>
@@ -4283,7 +4283,7 @@
         <v>52</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G37" s="4" t="s">
         <v>50</v>
@@ -4304,7 +4304,7 @@
         <v>333</v>
       </c>
       <c r="M37" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N37" s="4" t="s">
         <v>277</v>
@@ -4324,7 +4324,7 @@
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>50</v>
@@ -4339,7 +4339,7 @@
         <v>53</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>50</v>
@@ -4360,7 +4360,7 @@
         <v>333</v>
       </c>
       <c r="M38" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N38" s="4" t="s">
         <v>277</v>
@@ -4380,7 +4380,7 @@
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>54</v>
@@ -4395,7 +4395,7 @@
         <v>56</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>54</v>
@@ -4416,7 +4416,7 @@
         <v>345</v>
       </c>
       <c r="M39" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N39" s="4" t="s">
         <v>9</v>
@@ -4436,7 +4436,7 @@
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>54</v>
@@ -4451,7 +4451,7 @@
         <v>57</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>54</v>
@@ -4472,7 +4472,7 @@
         <v>345</v>
       </c>
       <c r="M40" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N40" s="4" t="s">
         <v>9</v>
@@ -4492,7 +4492,7 @@
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>58</v>
@@ -4507,7 +4507,7 @@
         <v>60</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G41" s="4" t="s">
         <v>58</v>
@@ -4528,7 +4528,7 @@
         <v>329</v>
       </c>
       <c r="M41" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N41" s="4" t="s">
         <v>145</v>
@@ -4548,7 +4548,7 @@
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>58</v>
@@ -4563,7 +4563,7 @@
         <v>61</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G42" s="4" t="s">
         <v>58</v>
@@ -4584,7 +4584,7 @@
         <v>329</v>
       </c>
       <c r="M42" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N42" s="4" t="s">
         <v>146</v>
@@ -4604,7 +4604,7 @@
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>62</v>
@@ -4619,7 +4619,7 @@
         <v>9</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G43" s="4" t="s">
         <v>62</v>
@@ -4640,7 +4640,7 @@
         <v>333</v>
       </c>
       <c r="M43" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N43" s="4" t="s">
         <v>135</v>
@@ -4660,7 +4660,7 @@
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>62</v>
@@ -4675,7 +4675,7 @@
         <v>65</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>62</v>
@@ -4696,7 +4696,7 @@
         <v>336</v>
       </c>
       <c r="M44" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N44" s="4" t="s">
         <v>135</v>
@@ -4716,7 +4716,7 @@
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>62</v>
@@ -4731,7 +4731,7 @@
         <v>16</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G45" s="4" t="s">
         <v>62</v>
@@ -4752,7 +4752,7 @@
         <v>336</v>
       </c>
       <c r="M45" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N45" s="4" t="s">
         <v>135</v>
@@ -4772,7 +4772,7 @@
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>62</v>
@@ -4787,7 +4787,7 @@
         <v>17</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G46" s="4" t="s">
         <v>62</v>
@@ -4808,7 +4808,7 @@
         <v>336</v>
       </c>
       <c r="M46" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N46" s="4" t="s">
         <v>135</v>
@@ -4828,7 +4828,7 @@
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>66</v>
@@ -4843,7 +4843,7 @@
         <v>9</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G47" s="4" t="s">
         <v>66</v>
@@ -4864,7 +4864,7 @@
         <v>333</v>
       </c>
       <c r="M47" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N47" s="4" t="s">
         <v>135</v>
@@ -4884,7 +4884,7 @@
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>67</v>
@@ -4899,7 +4899,7 @@
         <v>9</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G48" s="4" t="s">
         <v>68</v>
@@ -4920,7 +4920,7 @@
         <v>333</v>
       </c>
       <c r="M48" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N48" s="4" t="s">
         <v>148</v>
@@ -4940,7 +4940,7 @@
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>67</v>
@@ -4955,7 +4955,7 @@
         <v>9</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G49" s="4" t="s">
         <v>68</v>
@@ -4976,7 +4976,7 @@
         <v>341</v>
       </c>
       <c r="M49" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N49" s="4" t="s">
         <v>9</v>
@@ -4996,7 +4996,7 @@
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>68</v>
@@ -5011,7 +5011,7 @@
         <v>9</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G50" s="4" t="s">
         <v>68</v>
@@ -5032,7 +5032,7 @@
         <v>333</v>
       </c>
       <c r="M50" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N50" s="4" t="s">
         <v>148</v>
@@ -5052,7 +5052,7 @@
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>68</v>
@@ -5067,7 +5067,7 @@
         <v>9</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G51" s="4" t="s">
         <v>68</v>
@@ -5088,7 +5088,7 @@
         <v>341</v>
       </c>
       <c r="M51" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N51" s="4" t="s">
         <v>9</v>
@@ -5108,7 +5108,7 @@
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>69</v>
@@ -5123,7 +5123,7 @@
         <v>56</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G52" s="4" t="s">
         <v>69</v>
@@ -5144,7 +5144,7 @@
         <v>331</v>
       </c>
       <c r="M52" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N52" s="4" t="s">
         <v>284</v>
@@ -5164,7 +5164,7 @@
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>69</v>
@@ -5179,7 +5179,7 @@
         <v>57</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G53" s="4" t="s">
         <v>69</v>
@@ -5200,7 +5200,7 @@
         <v>331</v>
       </c>
       <c r="M53" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N53" s="4" t="s">
         <v>284</v>
@@ -5220,7 +5220,7 @@
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>71</v>
@@ -5235,7 +5235,7 @@
         <v>73</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G54" s="4" t="s">
         <v>71</v>
@@ -5256,10 +5256,10 @@
         <v>331</v>
       </c>
       <c r="M54" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="N54" s="4" t="s">
         <v>360</v>
-      </c>
-      <c r="N54" s="4" t="s">
-        <v>361</v>
       </c>
       <c r="O54" s="4" t="s">
         <v>136</v>
@@ -5276,7 +5276,7 @@
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>71</v>
@@ -5291,7 +5291,7 @@
         <v>74</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G55" s="4" t="s">
         <v>71</v>
@@ -5312,10 +5312,10 @@
         <v>331</v>
       </c>
       <c r="M55" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="N55" s="4" t="s">
         <v>360</v>
-      </c>
-      <c r="N55" s="4" t="s">
-        <v>361</v>
       </c>
       <c r="O55" s="4" t="s">
         <v>136</v>
@@ -5332,7 +5332,7 @@
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>71</v>
@@ -5347,7 +5347,7 @@
         <v>75</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G56" s="4" t="s">
         <v>71</v>
@@ -5368,10 +5368,10 @@
         <v>331</v>
       </c>
       <c r="M56" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="N56" s="4" t="s">
         <v>360</v>
-      </c>
-      <c r="N56" s="4" t="s">
-        <v>361</v>
       </c>
       <c r="O56" s="4" t="s">
         <v>136</v>
@@ -5388,7 +5388,7 @@
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>71</v>
@@ -5403,7 +5403,7 @@
         <v>76</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G57" s="4" t="s">
         <v>71</v>
@@ -5424,10 +5424,10 @@
         <v>331</v>
       </c>
       <c r="M57" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="N57" s="4" t="s">
         <v>360</v>
-      </c>
-      <c r="N57" s="4" t="s">
-        <v>361</v>
       </c>
       <c r="O57" s="4" t="s">
         <v>136</v>
@@ -5444,7 +5444,7 @@
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>71</v>
@@ -5459,7 +5459,7 @@
         <v>73</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G58" s="4" t="s">
         <v>71</v>
@@ -5480,10 +5480,10 @@
         <v>331</v>
       </c>
       <c r="M58" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="N58" s="4" t="s">
         <v>360</v>
-      </c>
-      <c r="N58" s="4" t="s">
-        <v>361</v>
       </c>
       <c r="O58" s="4" t="s">
         <v>136</v>
@@ -5500,7 +5500,7 @@
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>71</v>
@@ -5515,7 +5515,7 @@
         <v>74</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G59" s="4" t="s">
         <v>71</v>
@@ -5536,10 +5536,10 @@
         <v>331</v>
       </c>
       <c r="M59" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="N59" s="4" t="s">
         <v>360</v>
-      </c>
-      <c r="N59" s="4" t="s">
-        <v>361</v>
       </c>
       <c r="O59" s="4" t="s">
         <v>136</v>
@@ -5556,7 +5556,7 @@
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>71</v>
@@ -5571,7 +5571,7 @@
         <v>75</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G60" s="4" t="s">
         <v>71</v>
@@ -5592,10 +5592,10 @@
         <v>331</v>
       </c>
       <c r="M60" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="N60" s="4" t="s">
         <v>360</v>
-      </c>
-      <c r="N60" s="4" t="s">
-        <v>361</v>
       </c>
       <c r="O60" s="4" t="s">
         <v>136</v>
@@ -5612,7 +5612,7 @@
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>71</v>
@@ -5627,7 +5627,7 @@
         <v>76</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G61" s="4" t="s">
         <v>71</v>
@@ -5648,10 +5648,10 @@
         <v>331</v>
       </c>
       <c r="M61" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="N61" s="4" t="s">
         <v>360</v>
-      </c>
-      <c r="N61" s="4" t="s">
-        <v>361</v>
       </c>
       <c r="O61" s="4" t="s">
         <v>136</v>
@@ -5668,7 +5668,7 @@
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B62" s="4" t="s">
         <v>77</v>
@@ -5683,7 +5683,7 @@
         <v>9</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G62" s="4" t="s">
         <v>77</v>
@@ -5704,7 +5704,7 @@
         <v>333</v>
       </c>
       <c r="M62" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N62" s="4" t="s">
         <v>284</v>
@@ -5724,7 +5724,7 @@
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B63" s="4" t="s">
         <v>77</v>
@@ -5739,7 +5739,7 @@
         <v>65</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G63" s="4" t="s">
         <v>77</v>
@@ -5760,7 +5760,7 @@
         <v>330</v>
       </c>
       <c r="M63" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N63" s="4" t="s">
         <v>284</v>
@@ -5780,7 +5780,7 @@
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B64" s="4" t="s">
         <v>77</v>
@@ -5795,7 +5795,7 @@
         <v>16</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G64" s="4" t="s">
         <v>77</v>
@@ -5816,7 +5816,7 @@
         <v>330</v>
       </c>
       <c r="M64" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N64" s="4" t="s">
         <v>284</v>
@@ -5836,7 +5836,7 @@
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B65" s="4" t="s">
         <v>77</v>
@@ -5851,7 +5851,7 @@
         <v>17</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G65" s="4" t="s">
         <v>77</v>
@@ -5872,7 +5872,7 @@
         <v>330</v>
       </c>
       <c r="M65" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N65" s="4" t="s">
         <v>284</v>
@@ -5892,7 +5892,7 @@
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B66" s="4" t="s">
         <v>79</v>
@@ -5907,7 +5907,7 @@
         <v>9</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G66" s="4" t="s">
         <v>79</v>
@@ -5928,7 +5928,7 @@
         <v>335</v>
       </c>
       <c r="M66" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N66" s="4" t="s">
         <v>285</v>
@@ -5948,7 +5948,7 @@
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B67" s="4" t="s">
         <v>80</v>
@@ -5963,7 +5963,7 @@
         <v>9</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G67" s="4" t="s">
         <v>80</v>
@@ -5984,7 +5984,7 @@
         <v>335</v>
       </c>
       <c r="M67" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N67" s="4" t="s">
         <v>285</v>
@@ -6004,7 +6004,7 @@
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B68" s="4" t="s">
         <v>80</v>
@@ -6019,7 +6019,7 @@
         <v>9</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G68" s="4" t="s">
         <v>80</v>
@@ -6040,7 +6040,7 @@
         <v>342</v>
       </c>
       <c r="M68" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N68" s="4" t="s">
         <v>9</v>
@@ -6060,7 +6060,7 @@
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B69" s="4" t="s">
         <v>82</v>
@@ -6075,7 +6075,7 @@
         <v>84</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G69" s="4" t="s">
         <v>82</v>
@@ -6096,7 +6096,7 @@
         <v>332</v>
       </c>
       <c r="M69" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N69" s="4" t="s">
         <v>284</v>
@@ -6116,7 +6116,7 @@
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B70" s="4" t="s">
         <v>82</v>
@@ -6131,7 +6131,7 @@
         <v>84</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G70" s="4" t="s">
         <v>82</v>
@@ -6152,7 +6152,7 @@
         <v>332</v>
       </c>
       <c r="M70" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N70" s="4" t="s">
         <v>284</v>
@@ -6172,7 +6172,7 @@
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B71" s="4" t="s">
         <v>85</v>
@@ -6187,7 +6187,7 @@
         <v>87</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G71" s="4" t="s">
         <v>85</v>
@@ -6208,10 +6208,10 @@
         <v>331</v>
       </c>
       <c r="M71" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="N71" s="4" t="s">
         <v>360</v>
-      </c>
-      <c r="N71" s="4" t="s">
-        <v>361</v>
       </c>
       <c r="O71" s="4" t="s">
         <v>136</v>
@@ -6228,7 +6228,7 @@
     </row>
     <row r="72" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B72" s="4" t="s">
         <v>85</v>
@@ -6243,7 +6243,7 @@
         <v>88</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G72" s="4" t="s">
         <v>85</v>
@@ -6264,10 +6264,10 @@
         <v>331</v>
       </c>
       <c r="M72" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="N72" s="4" t="s">
         <v>360</v>
-      </c>
-      <c r="N72" s="4" t="s">
-        <v>361</v>
       </c>
       <c r="O72" s="4" t="s">
         <v>136</v>
@@ -6284,7 +6284,7 @@
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B73" s="4" t="s">
         <v>85</v>
@@ -6299,7 +6299,7 @@
         <v>89</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G73" s="4" t="s">
         <v>85</v>
@@ -6320,10 +6320,10 @@
         <v>331</v>
       </c>
       <c r="M73" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="N73" s="4" t="s">
         <v>360</v>
-      </c>
-      <c r="N73" s="4" t="s">
-        <v>361</v>
       </c>
       <c r="O73" s="4" t="s">
         <v>136</v>
@@ -6340,7 +6340,7 @@
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B74" s="4" t="s">
         <v>85</v>
@@ -6355,7 +6355,7 @@
         <v>90</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G74" s="4" t="s">
         <v>85</v>
@@ -6376,10 +6376,10 @@
         <v>331</v>
       </c>
       <c r="M74" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="N74" s="4" t="s">
         <v>360</v>
-      </c>
-      <c r="N74" s="4" t="s">
-        <v>361</v>
       </c>
       <c r="O74" s="4" t="s">
         <v>136</v>
@@ -6396,7 +6396,7 @@
     </row>
     <row r="75" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B75" s="4" t="s">
         <v>91</v>
@@ -6411,7 +6411,7 @@
         <v>30</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G75" s="4" t="s">
         <v>91</v>
@@ -6432,7 +6432,7 @@
         <v>333</v>
       </c>
       <c r="M75" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N75" s="4" t="s">
         <v>135</v>
@@ -6452,7 +6452,7 @@
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B76" s="4" t="s">
         <v>91</v>
@@ -6467,7 +6467,7 @@
         <v>31</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G76" s="4" t="s">
         <v>91</v>
@@ -6488,7 +6488,7 @@
         <v>333</v>
       </c>
       <c r="M76" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N76" s="4" t="s">
         <v>135</v>
@@ -6508,7 +6508,7 @@
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B77" s="4" t="s">
         <v>91</v>
@@ -6523,7 +6523,7 @@
         <v>92</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="G77" s="4" t="s">
         <v>91</v>
@@ -6544,7 +6544,7 @@
         <v>333</v>
       </c>
       <c r="M77" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N77" s="4" t="s">
         <v>135</v>

</xml_diff>

<commit_message>
20T to 21 T update fiscal year.
</commit_message>
<xml_diff>
--- a/data-raw/snu_x_im_distribution_configuration/20Tto21TMap.xlsx
+++ b/data-raw/snu_x_im_distribution_configuration/20Tto21TMap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/snu_x_im_distribution_configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{DF270AA2-15E0-3E47-B4E3-CC419906039A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{C9692DBF-18D3-D14A-A68F-7A89348D1358}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="460" windowWidth="25600" windowHeight="20020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1113,9 +1113,6 @@
     <t>pe</t>
   </si>
   <si>
-    <t>2018Oct</t>
-  </si>
-  <si>
     <t>&lt;15/&gt;15</t>
   </si>
   <si>
@@ -1351,6 +1348,9 @@
   </si>
   <si>
     <t>DE_GROUP-XUA8pDYjPsw</t>
+  </si>
+  <si>
+    <t>2019Oct</t>
   </si>
 </sst>
 </file>
@@ -2224,8 +2224,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="E36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M66" sqref="M66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2252,7 +2252,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>298</v>
@@ -2308,7 +2308,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>10</v>
@@ -2323,7 +2323,7 @@
         <v>12</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>10</v>
@@ -2344,7 +2344,7 @@
         <v>355</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>9</v>
@@ -2364,7 +2364,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>10</v>
@@ -2379,7 +2379,7 @@
         <v>13</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>10</v>
@@ -2400,7 +2400,7 @@
         <v>355</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N3" s="4" t="s">
         <v>9</v>
@@ -2420,7 +2420,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>14</v>
@@ -2435,7 +2435,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>42</v>
@@ -2456,7 +2456,7 @@
         <v>339</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>137</v>
@@ -2476,7 +2476,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>14</v>
@@ -2491,7 +2491,7 @@
         <v>17</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>42</v>
@@ -2512,7 +2512,7 @@
         <v>339</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N5" s="4" t="s">
         <v>137</v>
@@ -2532,7 +2532,7 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>18</v>
@@ -2547,7 +2547,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>42</v>
@@ -2568,7 +2568,7 @@
         <v>338</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N6" s="4" t="s">
         <v>137</v>
@@ -2588,7 +2588,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>18</v>
@@ -2603,7 +2603,7 @@
         <v>17</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>42</v>
@@ -2624,7 +2624,7 @@
         <v>338</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N7" s="4" t="s">
         <v>137</v>
@@ -2644,7 +2644,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>24</v>
@@ -2659,7 +2659,7 @@
         <v>26</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>24</v>
@@ -2680,7 +2680,7 @@
         <v>334</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N8" s="4" t="s">
         <v>135</v>
@@ -2700,7 +2700,7 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>24</v>
@@ -2715,7 +2715,7 @@
         <v>28</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>24</v>
@@ -2736,7 +2736,7 @@
         <v>334</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N9" s="4" t="s">
         <v>135</v>
@@ -2756,7 +2756,7 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>29</v>
@@ -2771,7 +2771,7 @@
         <v>30</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>42</v>
@@ -2792,7 +2792,7 @@
         <v>337</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N10" s="4" t="s">
         <v>137</v>
@@ -2812,7 +2812,7 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>29</v>
@@ -2827,7 +2827,7 @@
         <v>31</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>42</v>
@@ -2848,7 +2848,7 @@
         <v>337</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N11" s="4" t="s">
         <v>137</v>
@@ -2868,7 +2868,7 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>32</v>
@@ -2883,7 +2883,7 @@
         <v>30</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>42</v>
@@ -2904,7 +2904,7 @@
         <v>340</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N12" s="4" t="s">
         <v>137</v>
@@ -2924,7 +2924,7 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>32</v>
@@ -2939,7 +2939,7 @@
         <v>31</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>42</v>
@@ -2960,7 +2960,7 @@
         <v>340</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N13" s="4" t="s">
         <v>137</v>
@@ -2980,7 +2980,7 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>33</v>
@@ -2995,7 +2995,7 @@
         <v>30</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>42</v>
@@ -3016,7 +3016,7 @@
         <v>344</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N14" s="4" t="s">
         <v>139</v>
@@ -3036,7 +3036,7 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>33</v>
@@ -3051,7 +3051,7 @@
         <v>31</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>42</v>
@@ -3072,7 +3072,7 @@
         <v>344</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N15" s="4" t="s">
         <v>139</v>
@@ -3092,7 +3092,7 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>34</v>
@@ -3107,7 +3107,7 @@
         <v>30</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>42</v>
@@ -3128,7 +3128,7 @@
         <v>356</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N16" s="4" t="s">
         <v>137</v>
@@ -3148,7 +3148,7 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>34</v>
@@ -3163,7 +3163,7 @@
         <v>31</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>42</v>
@@ -3184,7 +3184,7 @@
         <v>356</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N17" s="4" t="s">
         <v>137</v>
@@ -3204,7 +3204,7 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>35</v>
@@ -3219,7 +3219,7 @@
         <v>30</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>42</v>
@@ -3240,7 +3240,7 @@
         <v>347</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N18" s="4" t="s">
         <v>137</v>
@@ -3260,7 +3260,7 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>35</v>
@@ -3275,7 +3275,7 @@
         <v>31</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>42</v>
@@ -3296,7 +3296,7 @@
         <v>347</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N19" s="4" t="s">
         <v>137</v>
@@ -3316,7 +3316,7 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>36</v>
@@ -3331,7 +3331,7 @@
         <v>30</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>42</v>
@@ -3352,7 +3352,7 @@
         <v>348</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N20" s="4" t="s">
         <v>137</v>
@@ -3372,7 +3372,7 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>36</v>
@@ -3387,7 +3387,7 @@
         <v>31</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>42</v>
@@ -3408,7 +3408,7 @@
         <v>348</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N21" s="4" t="s">
         <v>137</v>
@@ -3428,7 +3428,7 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>37</v>
@@ -3443,7 +3443,7 @@
         <v>30</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>42</v>
@@ -3464,7 +3464,7 @@
         <v>349</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N22" s="4" t="s">
         <v>139</v>
@@ -3484,7 +3484,7 @@
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>37</v>
@@ -3499,7 +3499,7 @@
         <v>31</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>42</v>
@@ -3520,7 +3520,7 @@
         <v>349</v>
       </c>
       <c r="M23" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N23" s="4" t="s">
         <v>139</v>
@@ -3540,7 +3540,7 @@
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>38</v>
@@ -3555,7 +3555,7 @@
         <v>30</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>42</v>
@@ -3576,7 +3576,7 @@
         <v>350</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N24" s="4" t="s">
         <v>137</v>
@@ -3596,7 +3596,7 @@
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>38</v>
@@ -3611,7 +3611,7 @@
         <v>31</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>42</v>
@@ -3632,7 +3632,7 @@
         <v>350</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N25" s="4" t="s">
         <v>137</v>
@@ -3652,7 +3652,7 @@
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>39</v>
@@ -3667,7 +3667,7 @@
         <v>30</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>42</v>
@@ -3688,7 +3688,7 @@
         <v>352</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N26" s="4" t="s">
         <v>137</v>
@@ -3708,7 +3708,7 @@
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>39</v>
@@ -3723,7 +3723,7 @@
         <v>31</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>42</v>
@@ -3744,7 +3744,7 @@
         <v>352</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N27" s="4" t="s">
         <v>137</v>
@@ -3764,7 +3764,7 @@
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>40</v>
@@ -3779,7 +3779,7 @@
         <v>30</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>42</v>
@@ -3800,7 +3800,7 @@
         <v>353</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N28" s="4" t="s">
         <v>137</v>
@@ -3820,7 +3820,7 @@
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>40</v>
@@ -3835,7 +3835,7 @@
         <v>31</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>42</v>
@@ -3856,7 +3856,7 @@
         <v>353</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N29" s="4" t="s">
         <v>137</v>
@@ -3876,7 +3876,7 @@
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>41</v>
@@ -3891,7 +3891,7 @@
         <v>30</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>42</v>
@@ -3912,7 +3912,7 @@
         <v>354</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N30" s="4" t="s">
         <v>137</v>
@@ -3932,7 +3932,7 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>41</v>
@@ -3947,7 +3947,7 @@
         <v>31</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>42</v>
@@ -3968,7 +3968,7 @@
         <v>354</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N31" s="4" t="s">
         <v>137</v>
@@ -3988,7 +3988,7 @@
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>42</v>
@@ -4003,7 +4003,7 @@
         <v>30</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>42</v>
@@ -4024,7 +4024,7 @@
         <v>343</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N32" s="4" t="s">
         <v>9</v>
@@ -4044,7 +4044,7 @@
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>42</v>
@@ -4059,7 +4059,7 @@
         <v>31</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>42</v>
@@ -4080,7 +4080,7 @@
         <v>343</v>
       </c>
       <c r="M33" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N33" s="4" t="s">
         <v>9</v>
@@ -4100,7 +4100,7 @@
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>44</v>
@@ -4115,7 +4115,7 @@
         <v>9</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>44</v>
@@ -4136,7 +4136,7 @@
         <v>351</v>
       </c>
       <c r="M34" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N34" s="4" t="s">
         <v>9</v>
@@ -4156,7 +4156,7 @@
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>46</v>
@@ -4171,7 +4171,7 @@
         <v>9</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>46</v>
@@ -4192,7 +4192,7 @@
         <v>341</v>
       </c>
       <c r="M35" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N35" s="4" t="s">
         <v>9</v>
@@ -4212,7 +4212,7 @@
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>48</v>
@@ -4227,7 +4227,7 @@
         <v>9</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G36" s="4" t="s">
         <v>48</v>
@@ -4248,7 +4248,7 @@
         <v>346</v>
       </c>
       <c r="M36" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N36" s="4" t="s">
         <v>9</v>
@@ -4268,7 +4268,7 @@
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>50</v>
@@ -4283,7 +4283,7 @@
         <v>52</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G37" s="4" t="s">
         <v>50</v>
@@ -4304,7 +4304,7 @@
         <v>333</v>
       </c>
       <c r="M37" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N37" s="4" t="s">
         <v>277</v>
@@ -4324,7 +4324,7 @@
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>50</v>
@@ -4339,7 +4339,7 @@
         <v>53</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>50</v>
@@ -4360,7 +4360,7 @@
         <v>333</v>
       </c>
       <c r="M38" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N38" s="4" t="s">
         <v>277</v>
@@ -4380,7 +4380,7 @@
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>54</v>
@@ -4395,7 +4395,7 @@
         <v>56</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>54</v>
@@ -4416,7 +4416,7 @@
         <v>345</v>
       </c>
       <c r="M39" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N39" s="4" t="s">
         <v>9</v>
@@ -4436,7 +4436,7 @@
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>54</v>
@@ -4451,7 +4451,7 @@
         <v>57</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>54</v>
@@ -4472,7 +4472,7 @@
         <v>345</v>
       </c>
       <c r="M40" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N40" s="4" t="s">
         <v>9</v>
@@ -4492,7 +4492,7 @@
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>58</v>
@@ -4507,7 +4507,7 @@
         <v>60</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G41" s="4" t="s">
         <v>58</v>
@@ -4528,7 +4528,7 @@
         <v>329</v>
       </c>
       <c r="M41" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N41" s="4" t="s">
         <v>145</v>
@@ -4548,7 +4548,7 @@
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>58</v>
@@ -4563,7 +4563,7 @@
         <v>61</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G42" s="4" t="s">
         <v>58</v>
@@ -4584,7 +4584,7 @@
         <v>329</v>
       </c>
       <c r="M42" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N42" s="4" t="s">
         <v>146</v>
@@ -4604,7 +4604,7 @@
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>62</v>
@@ -4619,7 +4619,7 @@
         <v>9</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G43" s="4" t="s">
         <v>62</v>
@@ -4640,7 +4640,7 @@
         <v>333</v>
       </c>
       <c r="M43" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N43" s="4" t="s">
         <v>135</v>
@@ -4660,7 +4660,7 @@
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>62</v>
@@ -4675,7 +4675,7 @@
         <v>65</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>62</v>
@@ -4696,7 +4696,7 @@
         <v>336</v>
       </c>
       <c r="M44" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N44" s="4" t="s">
         <v>135</v>
@@ -4716,7 +4716,7 @@
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>62</v>
@@ -4731,7 +4731,7 @@
         <v>16</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G45" s="4" t="s">
         <v>62</v>
@@ -4752,7 +4752,7 @@
         <v>336</v>
       </c>
       <c r="M45" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N45" s="4" t="s">
         <v>135</v>
@@ -4772,7 +4772,7 @@
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>62</v>
@@ -4787,7 +4787,7 @@
         <v>17</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G46" s="4" t="s">
         <v>62</v>
@@ -4808,7 +4808,7 @@
         <v>336</v>
       </c>
       <c r="M46" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N46" s="4" t="s">
         <v>135</v>
@@ -4828,7 +4828,7 @@
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>66</v>
@@ -4843,7 +4843,7 @@
         <v>9</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G47" s="4" t="s">
         <v>66</v>
@@ -4864,7 +4864,7 @@
         <v>333</v>
       </c>
       <c r="M47" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N47" s="4" t="s">
         <v>135</v>
@@ -4884,7 +4884,7 @@
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>67</v>
@@ -4899,7 +4899,7 @@
         <v>9</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G48" s="4" t="s">
         <v>68</v>
@@ -4920,7 +4920,7 @@
         <v>333</v>
       </c>
       <c r="M48" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N48" s="4" t="s">
         <v>148</v>
@@ -4940,7 +4940,7 @@
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>67</v>
@@ -4955,7 +4955,7 @@
         <v>9</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G49" s="4" t="s">
         <v>68</v>
@@ -4976,7 +4976,7 @@
         <v>341</v>
       </c>
       <c r="M49" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N49" s="4" t="s">
         <v>9</v>
@@ -4996,7 +4996,7 @@
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>68</v>
@@ -5011,7 +5011,7 @@
         <v>9</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G50" s="4" t="s">
         <v>68</v>
@@ -5032,7 +5032,7 @@
         <v>333</v>
       </c>
       <c r="M50" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N50" s="4" t="s">
         <v>148</v>
@@ -5052,7 +5052,7 @@
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>68</v>
@@ -5067,7 +5067,7 @@
         <v>9</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G51" s="4" t="s">
         <v>68</v>
@@ -5088,7 +5088,7 @@
         <v>341</v>
       </c>
       <c r="M51" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N51" s="4" t="s">
         <v>9</v>
@@ -5108,7 +5108,7 @@
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>69</v>
@@ -5123,7 +5123,7 @@
         <v>56</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G52" s="4" t="s">
         <v>69</v>
@@ -5144,7 +5144,7 @@
         <v>331</v>
       </c>
       <c r="M52" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N52" s="4" t="s">
         <v>284</v>
@@ -5164,7 +5164,7 @@
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>69</v>
@@ -5179,7 +5179,7 @@
         <v>57</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G53" s="4" t="s">
         <v>69</v>
@@ -5200,7 +5200,7 @@
         <v>331</v>
       </c>
       <c r="M53" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N53" s="4" t="s">
         <v>284</v>
@@ -5220,7 +5220,7 @@
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>71</v>
@@ -5235,7 +5235,7 @@
         <v>73</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G54" s="4" t="s">
         <v>71</v>
@@ -5256,10 +5256,10 @@
         <v>331</v>
       </c>
       <c r="M54" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="N54" s="4" t="s">
         <v>359</v>
-      </c>
-      <c r="N54" s="4" t="s">
-        <v>360</v>
       </c>
       <c r="O54" s="4" t="s">
         <v>136</v>
@@ -5276,7 +5276,7 @@
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>71</v>
@@ -5291,7 +5291,7 @@
         <v>74</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G55" s="4" t="s">
         <v>71</v>
@@ -5312,10 +5312,10 @@
         <v>331</v>
       </c>
       <c r="M55" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="N55" s="4" t="s">
         <v>359</v>
-      </c>
-      <c r="N55" s="4" t="s">
-        <v>360</v>
       </c>
       <c r="O55" s="4" t="s">
         <v>136</v>
@@ -5332,7 +5332,7 @@
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>71</v>
@@ -5347,7 +5347,7 @@
         <v>75</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G56" s="4" t="s">
         <v>71</v>
@@ -5368,10 +5368,10 @@
         <v>331</v>
       </c>
       <c r="M56" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="N56" s="4" t="s">
         <v>359</v>
-      </c>
-      <c r="N56" s="4" t="s">
-        <v>360</v>
       </c>
       <c r="O56" s="4" t="s">
         <v>136</v>
@@ -5388,7 +5388,7 @@
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>71</v>
@@ -5403,7 +5403,7 @@
         <v>76</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G57" s="4" t="s">
         <v>71</v>
@@ -5424,10 +5424,10 @@
         <v>331</v>
       </c>
       <c r="M57" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="N57" s="4" t="s">
         <v>359</v>
-      </c>
-      <c r="N57" s="4" t="s">
-        <v>360</v>
       </c>
       <c r="O57" s="4" t="s">
         <v>136</v>
@@ -5444,7 +5444,7 @@
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>71</v>
@@ -5459,7 +5459,7 @@
         <v>73</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G58" s="4" t="s">
         <v>71</v>
@@ -5480,10 +5480,10 @@
         <v>331</v>
       </c>
       <c r="M58" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="N58" s="4" t="s">
         <v>359</v>
-      </c>
-      <c r="N58" s="4" t="s">
-        <v>360</v>
       </c>
       <c r="O58" s="4" t="s">
         <v>136</v>
@@ -5500,7 +5500,7 @@
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>71</v>
@@ -5515,7 +5515,7 @@
         <v>74</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G59" s="4" t="s">
         <v>71</v>
@@ -5536,10 +5536,10 @@
         <v>331</v>
       </c>
       <c r="M59" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="N59" s="4" t="s">
         <v>359</v>
-      </c>
-      <c r="N59" s="4" t="s">
-        <v>360</v>
       </c>
       <c r="O59" s="4" t="s">
         <v>136</v>
@@ -5556,7 +5556,7 @@
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>71</v>
@@ -5571,7 +5571,7 @@
         <v>75</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G60" s="4" t="s">
         <v>71</v>
@@ -5592,10 +5592,10 @@
         <v>331</v>
       </c>
       <c r="M60" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="N60" s="4" t="s">
         <v>359</v>
-      </c>
-      <c r="N60" s="4" t="s">
-        <v>360</v>
       </c>
       <c r="O60" s="4" t="s">
         <v>136</v>
@@ -5612,7 +5612,7 @@
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>71</v>
@@ -5627,7 +5627,7 @@
         <v>76</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G61" s="4" t="s">
         <v>71</v>
@@ -5648,10 +5648,10 @@
         <v>331</v>
       </c>
       <c r="M61" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="N61" s="4" t="s">
         <v>359</v>
-      </c>
-      <c r="N61" s="4" t="s">
-        <v>360</v>
       </c>
       <c r="O61" s="4" t="s">
         <v>136</v>
@@ -5668,7 +5668,7 @@
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B62" s="4" t="s">
         <v>77</v>
@@ -5683,7 +5683,7 @@
         <v>9</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G62" s="4" t="s">
         <v>77</v>
@@ -5704,7 +5704,7 @@
         <v>333</v>
       </c>
       <c r="M62" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N62" s="4" t="s">
         <v>284</v>
@@ -5724,7 +5724,7 @@
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B63" s="4" t="s">
         <v>77</v>
@@ -5739,7 +5739,7 @@
         <v>65</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G63" s="4" t="s">
         <v>77</v>
@@ -5760,7 +5760,7 @@
         <v>330</v>
       </c>
       <c r="M63" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N63" s="4" t="s">
         <v>284</v>
@@ -5780,7 +5780,7 @@
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B64" s="4" t="s">
         <v>77</v>
@@ -5795,7 +5795,7 @@
         <v>16</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G64" s="4" t="s">
         <v>77</v>
@@ -5816,7 +5816,7 @@
         <v>330</v>
       </c>
       <c r="M64" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N64" s="4" t="s">
         <v>284</v>
@@ -5836,7 +5836,7 @@
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B65" s="4" t="s">
         <v>77</v>
@@ -5851,7 +5851,7 @@
         <v>17</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G65" s="4" t="s">
         <v>77</v>
@@ -5872,7 +5872,7 @@
         <v>330</v>
       </c>
       <c r="M65" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N65" s="4" t="s">
         <v>284</v>
@@ -5892,7 +5892,7 @@
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B66" s="4" t="s">
         <v>79</v>
@@ -5907,7 +5907,7 @@
         <v>9</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G66" s="4" t="s">
         <v>79</v>
@@ -5928,7 +5928,7 @@
         <v>335</v>
       </c>
       <c r="M66" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N66" s="4" t="s">
         <v>285</v>
@@ -5948,7 +5948,7 @@
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B67" s="4" t="s">
         <v>80</v>
@@ -5963,7 +5963,7 @@
         <v>9</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G67" s="4" t="s">
         <v>80</v>
@@ -5984,7 +5984,7 @@
         <v>335</v>
       </c>
       <c r="M67" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N67" s="4" t="s">
         <v>285</v>
@@ -6004,7 +6004,7 @@
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B68" s="4" t="s">
         <v>80</v>
@@ -6019,7 +6019,7 @@
         <v>9</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G68" s="4" t="s">
         <v>80</v>
@@ -6040,7 +6040,7 @@
         <v>342</v>
       </c>
       <c r="M68" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N68" s="4" t="s">
         <v>9</v>
@@ -6060,7 +6060,7 @@
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B69" s="4" t="s">
         <v>82</v>
@@ -6075,7 +6075,7 @@
         <v>84</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G69" s="4" t="s">
         <v>82</v>
@@ -6096,7 +6096,7 @@
         <v>332</v>
       </c>
       <c r="M69" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N69" s="4" t="s">
         <v>284</v>
@@ -6116,7 +6116,7 @@
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B70" s="4" t="s">
         <v>82</v>
@@ -6131,7 +6131,7 @@
         <v>84</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G70" s="4" t="s">
         <v>82</v>
@@ -6152,7 +6152,7 @@
         <v>332</v>
       </c>
       <c r="M70" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N70" s="4" t="s">
         <v>284</v>
@@ -6172,7 +6172,7 @@
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B71" s="4" t="s">
         <v>85</v>
@@ -6187,7 +6187,7 @@
         <v>87</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G71" s="4" t="s">
         <v>85</v>
@@ -6208,10 +6208,10 @@
         <v>331</v>
       </c>
       <c r="M71" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="N71" s="4" t="s">
         <v>359</v>
-      </c>
-      <c r="N71" s="4" t="s">
-        <v>360</v>
       </c>
       <c r="O71" s="4" t="s">
         <v>136</v>
@@ -6228,7 +6228,7 @@
     </row>
     <row r="72" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B72" s="4" t="s">
         <v>85</v>
@@ -6243,7 +6243,7 @@
         <v>88</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G72" s="4" t="s">
         <v>85</v>
@@ -6264,10 +6264,10 @@
         <v>331</v>
       </c>
       <c r="M72" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="N72" s="4" t="s">
         <v>359</v>
-      </c>
-      <c r="N72" s="4" t="s">
-        <v>360</v>
       </c>
       <c r="O72" s="4" t="s">
         <v>136</v>
@@ -6284,7 +6284,7 @@
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B73" s="4" t="s">
         <v>85</v>
@@ -6299,7 +6299,7 @@
         <v>89</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G73" s="4" t="s">
         <v>85</v>
@@ -6320,10 +6320,10 @@
         <v>331</v>
       </c>
       <c r="M73" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="N73" s="4" t="s">
         <v>359</v>
-      </c>
-      <c r="N73" s="4" t="s">
-        <v>360</v>
       </c>
       <c r="O73" s="4" t="s">
         <v>136</v>
@@ -6340,7 +6340,7 @@
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B74" s="4" t="s">
         <v>85</v>
@@ -6355,7 +6355,7 @@
         <v>90</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G74" s="4" t="s">
         <v>85</v>
@@ -6376,10 +6376,10 @@
         <v>331</v>
       </c>
       <c r="M74" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="N74" s="4" t="s">
         <v>359</v>
-      </c>
-      <c r="N74" s="4" t="s">
-        <v>360</v>
       </c>
       <c r="O74" s="4" t="s">
         <v>136</v>
@@ -6396,7 +6396,7 @@
     </row>
     <row r="75" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B75" s="4" t="s">
         <v>91</v>
@@ -6411,7 +6411,7 @@
         <v>30</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G75" s="4" t="s">
         <v>91</v>
@@ -6432,7 +6432,7 @@
         <v>333</v>
       </c>
       <c r="M75" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N75" s="4" t="s">
         <v>135</v>
@@ -6452,7 +6452,7 @@
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B76" s="4" t="s">
         <v>91</v>
@@ -6467,7 +6467,7 @@
         <v>31</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G76" s="4" t="s">
         <v>91</v>
@@ -6488,7 +6488,7 @@
         <v>333</v>
       </c>
       <c r="M76" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N76" s="4" t="s">
         <v>135</v>
@@ -6508,7 +6508,7 @@
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B77" s="4" t="s">
         <v>91</v>
@@ -6523,7 +6523,7 @@
         <v>92</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G77" s="4" t="s">
         <v>91</v>
@@ -6544,7 +6544,7 @@
         <v>333</v>
       </c>
       <c r="M77" s="4" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="N77" s="4" t="s">
         <v>135</v>

</xml_diff>

<commit_message>
update 20T to 21T map GEND_GBV indicator code
</commit_message>
<xml_diff>
--- a/data-raw/snu_x_im_distribution_configuration/20Tto21TMap.xlsx
+++ b/data-raw/snu_x_im_distribution_configuration/20Tto21TMap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/snu_x_im_distribution_configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{C9692DBF-18D3-D14A-A68F-7A89348D1358}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{AFDF73C7-49C1-8146-83C6-BCDA5B39A68D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="25600" windowHeight="20020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4860" yWindow="2080" windowWidth="25600" windowHeight="20020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="19Tto20TMap" sheetId="1" r:id="rId1"/>
@@ -1119,9 +1119,6 @@
     <t>GEND_GBV.N.ViolenceServiceType.T.physEmot</t>
   </si>
   <si>
-    <t>GEND_GBV.N.ViolenceServiceType.T.postRape</t>
-  </si>
-  <si>
     <t>HTS_SELF.N.HIVSelfTest.T.Unassisted</t>
   </si>
   <si>
@@ -1351,6 +1348,9 @@
   </si>
   <si>
     <t>2019Oct</t>
+  </si>
+  <si>
+    <t>GEND_GBV.N.ViolenceServiceType.T.Sexual</t>
   </si>
 </sst>
 </file>
@@ -2224,8 +2224,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E36" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M66" sqref="M66"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2252,7 +2252,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>298</v>
@@ -2323,7 +2323,7 @@
         <v>12</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>10</v>
@@ -2344,7 +2344,7 @@
         <v>355</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>9</v>
@@ -2364,7 +2364,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>361</v>
+        <v>438</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>10</v>
@@ -2379,7 +2379,7 @@
         <v>13</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>10</v>
@@ -2400,7 +2400,7 @@
         <v>355</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N3" s="4" t="s">
         <v>9</v>
@@ -2420,7 +2420,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>14</v>
@@ -2435,7 +2435,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>42</v>
@@ -2456,7 +2456,7 @@
         <v>339</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>137</v>
@@ -2476,7 +2476,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>14</v>
@@ -2491,7 +2491,7 @@
         <v>17</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>42</v>
@@ -2512,7 +2512,7 @@
         <v>339</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N5" s="4" t="s">
         <v>137</v>
@@ -2532,7 +2532,7 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>18</v>
@@ -2547,7 +2547,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>42</v>
@@ -2568,7 +2568,7 @@
         <v>338</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N6" s="4" t="s">
         <v>137</v>
@@ -2588,7 +2588,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>18</v>
@@ -2603,7 +2603,7 @@
         <v>17</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>42</v>
@@ -2624,7 +2624,7 @@
         <v>338</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N7" s="4" t="s">
         <v>137</v>
@@ -2644,7 +2644,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>24</v>
@@ -2659,7 +2659,7 @@
         <v>26</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>24</v>
@@ -2680,7 +2680,7 @@
         <v>334</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N8" s="4" t="s">
         <v>135</v>
@@ -2700,7 +2700,7 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>24</v>
@@ -2715,7 +2715,7 @@
         <v>28</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>24</v>
@@ -2736,7 +2736,7 @@
         <v>334</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N9" s="4" t="s">
         <v>135</v>
@@ -2756,7 +2756,7 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>29</v>
@@ -2771,7 +2771,7 @@
         <v>30</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>42</v>
@@ -2792,7 +2792,7 @@
         <v>337</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N10" s="4" t="s">
         <v>137</v>
@@ -2812,7 +2812,7 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>29</v>
@@ -2827,7 +2827,7 @@
         <v>31</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>42</v>
@@ -2848,7 +2848,7 @@
         <v>337</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N11" s="4" t="s">
         <v>137</v>
@@ -2868,7 +2868,7 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>32</v>
@@ -2883,7 +2883,7 @@
         <v>30</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>42</v>
@@ -2904,7 +2904,7 @@
         <v>340</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N12" s="4" t="s">
         <v>137</v>
@@ -2924,7 +2924,7 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>32</v>
@@ -2939,7 +2939,7 @@
         <v>31</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>42</v>
@@ -2960,7 +2960,7 @@
         <v>340</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N13" s="4" t="s">
         <v>137</v>
@@ -2980,7 +2980,7 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>33</v>
@@ -2995,7 +2995,7 @@
         <v>30</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>42</v>
@@ -3016,7 +3016,7 @@
         <v>344</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N14" s="4" t="s">
         <v>139</v>
@@ -3036,7 +3036,7 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>33</v>
@@ -3051,7 +3051,7 @@
         <v>31</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>42</v>
@@ -3072,7 +3072,7 @@
         <v>344</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N15" s="4" t="s">
         <v>139</v>
@@ -3092,7 +3092,7 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>34</v>
@@ -3107,7 +3107,7 @@
         <v>30</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>42</v>
@@ -3128,7 +3128,7 @@
         <v>356</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N16" s="4" t="s">
         <v>137</v>
@@ -3148,7 +3148,7 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>34</v>
@@ -3163,7 +3163,7 @@
         <v>31</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>42</v>
@@ -3184,7 +3184,7 @@
         <v>356</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N17" s="4" t="s">
         <v>137</v>
@@ -3204,7 +3204,7 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>35</v>
@@ -3219,7 +3219,7 @@
         <v>30</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>42</v>
@@ -3240,7 +3240,7 @@
         <v>347</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N18" s="4" t="s">
         <v>137</v>
@@ -3260,7 +3260,7 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>35</v>
@@ -3275,7 +3275,7 @@
         <v>31</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>42</v>
@@ -3296,7 +3296,7 @@
         <v>347</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N19" s="4" t="s">
         <v>137</v>
@@ -3316,7 +3316,7 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>36</v>
@@ -3331,7 +3331,7 @@
         <v>30</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>42</v>
@@ -3352,7 +3352,7 @@
         <v>348</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N20" s="4" t="s">
         <v>137</v>
@@ -3372,7 +3372,7 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>36</v>
@@ -3387,7 +3387,7 @@
         <v>31</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>42</v>
@@ -3408,7 +3408,7 @@
         <v>348</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N21" s="4" t="s">
         <v>137</v>
@@ -3428,7 +3428,7 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>37</v>
@@ -3443,7 +3443,7 @@
         <v>30</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>42</v>
@@ -3464,7 +3464,7 @@
         <v>349</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N22" s="4" t="s">
         <v>139</v>
@@ -3484,7 +3484,7 @@
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>37</v>
@@ -3499,7 +3499,7 @@
         <v>31</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>42</v>
@@ -3520,7 +3520,7 @@
         <v>349</v>
       </c>
       <c r="M23" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N23" s="4" t="s">
         <v>139</v>
@@ -3540,7 +3540,7 @@
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>38</v>
@@ -3555,7 +3555,7 @@
         <v>30</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>42</v>
@@ -3576,7 +3576,7 @@
         <v>350</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N24" s="4" t="s">
         <v>137</v>
@@ -3596,7 +3596,7 @@
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>38</v>
@@ -3611,7 +3611,7 @@
         <v>31</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>42</v>
@@ -3632,7 +3632,7 @@
         <v>350</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N25" s="4" t="s">
         <v>137</v>
@@ -3652,7 +3652,7 @@
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>39</v>
@@ -3667,7 +3667,7 @@
         <v>30</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>42</v>
@@ -3688,7 +3688,7 @@
         <v>352</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N26" s="4" t="s">
         <v>137</v>
@@ -3708,7 +3708,7 @@
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>39</v>
@@ -3723,7 +3723,7 @@
         <v>31</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>42</v>
@@ -3744,7 +3744,7 @@
         <v>352</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N27" s="4" t="s">
         <v>137</v>
@@ -3764,7 +3764,7 @@
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>40</v>
@@ -3779,7 +3779,7 @@
         <v>30</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>42</v>
@@ -3800,7 +3800,7 @@
         <v>353</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N28" s="4" t="s">
         <v>137</v>
@@ -3820,7 +3820,7 @@
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>40</v>
@@ -3835,7 +3835,7 @@
         <v>31</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>42</v>
@@ -3856,7 +3856,7 @@
         <v>353</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N29" s="4" t="s">
         <v>137</v>
@@ -3876,7 +3876,7 @@
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>41</v>
@@ -3891,7 +3891,7 @@
         <v>30</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>42</v>
@@ -3912,7 +3912,7 @@
         <v>354</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N30" s="4" t="s">
         <v>137</v>
@@ -3932,7 +3932,7 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>41</v>
@@ -3947,7 +3947,7 @@
         <v>31</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>42</v>
@@ -3968,7 +3968,7 @@
         <v>354</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N31" s="4" t="s">
         <v>137</v>
@@ -3988,7 +3988,7 @@
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>42</v>
@@ -4003,7 +4003,7 @@
         <v>30</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>42</v>
@@ -4024,7 +4024,7 @@
         <v>343</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N32" s="4" t="s">
         <v>9</v>
@@ -4044,7 +4044,7 @@
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>42</v>
@@ -4059,7 +4059,7 @@
         <v>31</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>42</v>
@@ -4080,7 +4080,7 @@
         <v>343</v>
       </c>
       <c r="M33" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N33" s="4" t="s">
         <v>9</v>
@@ -4100,7 +4100,7 @@
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>44</v>
@@ -4115,7 +4115,7 @@
         <v>9</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>44</v>
@@ -4136,7 +4136,7 @@
         <v>351</v>
       </c>
       <c r="M34" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N34" s="4" t="s">
         <v>9</v>
@@ -4156,7 +4156,7 @@
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>46</v>
@@ -4171,7 +4171,7 @@
         <v>9</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>46</v>
@@ -4192,7 +4192,7 @@
         <v>341</v>
       </c>
       <c r="M35" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N35" s="4" t="s">
         <v>9</v>
@@ -4212,7 +4212,7 @@
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>48</v>
@@ -4227,7 +4227,7 @@
         <v>9</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G36" s="4" t="s">
         <v>48</v>
@@ -4248,7 +4248,7 @@
         <v>346</v>
       </c>
       <c r="M36" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N36" s="4" t="s">
         <v>9</v>
@@ -4268,7 +4268,7 @@
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>50</v>
@@ -4283,7 +4283,7 @@
         <v>52</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G37" s="4" t="s">
         <v>50</v>
@@ -4304,7 +4304,7 @@
         <v>333</v>
       </c>
       <c r="M37" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N37" s="4" t="s">
         <v>277</v>
@@ -4324,7 +4324,7 @@
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>50</v>
@@ -4339,7 +4339,7 @@
         <v>53</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>50</v>
@@ -4360,7 +4360,7 @@
         <v>333</v>
       </c>
       <c r="M38" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N38" s="4" t="s">
         <v>277</v>
@@ -4380,7 +4380,7 @@
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>54</v>
@@ -4395,7 +4395,7 @@
         <v>56</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>54</v>
@@ -4416,7 +4416,7 @@
         <v>345</v>
       </c>
       <c r="M39" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N39" s="4" t="s">
         <v>9</v>
@@ -4436,7 +4436,7 @@
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>54</v>
@@ -4451,7 +4451,7 @@
         <v>57</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>54</v>
@@ -4472,7 +4472,7 @@
         <v>345</v>
       </c>
       <c r="M40" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N40" s="4" t="s">
         <v>9</v>
@@ -4492,7 +4492,7 @@
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>58</v>
@@ -4507,7 +4507,7 @@
         <v>60</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G41" s="4" t="s">
         <v>58</v>
@@ -4528,7 +4528,7 @@
         <v>329</v>
       </c>
       <c r="M41" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N41" s="4" t="s">
         <v>145</v>
@@ -4548,7 +4548,7 @@
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>58</v>
@@ -4563,7 +4563,7 @@
         <v>61</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G42" s="4" t="s">
         <v>58</v>
@@ -4584,7 +4584,7 @@
         <v>329</v>
       </c>
       <c r="M42" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N42" s="4" t="s">
         <v>146</v>
@@ -4604,7 +4604,7 @@
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>62</v>
@@ -4619,7 +4619,7 @@
         <v>9</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G43" s="4" t="s">
         <v>62</v>
@@ -4640,7 +4640,7 @@
         <v>333</v>
       </c>
       <c r="M43" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N43" s="4" t="s">
         <v>135</v>
@@ -4660,7 +4660,7 @@
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>62</v>
@@ -4675,7 +4675,7 @@
         <v>65</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>62</v>
@@ -4696,7 +4696,7 @@
         <v>336</v>
       </c>
       <c r="M44" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N44" s="4" t="s">
         <v>135</v>
@@ -4716,7 +4716,7 @@
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>62</v>
@@ -4731,7 +4731,7 @@
         <v>16</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G45" s="4" t="s">
         <v>62</v>
@@ -4752,7 +4752,7 @@
         <v>336</v>
       </c>
       <c r="M45" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N45" s="4" t="s">
         <v>135</v>
@@ -4772,7 +4772,7 @@
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>62</v>
@@ -4787,7 +4787,7 @@
         <v>17</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G46" s="4" t="s">
         <v>62</v>
@@ -4808,7 +4808,7 @@
         <v>336</v>
       </c>
       <c r="M46" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N46" s="4" t="s">
         <v>135</v>
@@ -4828,7 +4828,7 @@
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>66</v>
@@ -4843,7 +4843,7 @@
         <v>9</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G47" s="4" t="s">
         <v>66</v>
@@ -4864,7 +4864,7 @@
         <v>333</v>
       </c>
       <c r="M47" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N47" s="4" t="s">
         <v>135</v>
@@ -4884,7 +4884,7 @@
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>67</v>
@@ -4899,7 +4899,7 @@
         <v>9</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G48" s="4" t="s">
         <v>68</v>
@@ -4920,7 +4920,7 @@
         <v>333</v>
       </c>
       <c r="M48" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N48" s="4" t="s">
         <v>148</v>
@@ -4940,7 +4940,7 @@
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>67</v>
@@ -4955,7 +4955,7 @@
         <v>9</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G49" s="4" t="s">
         <v>68</v>
@@ -4976,7 +4976,7 @@
         <v>341</v>
       </c>
       <c r="M49" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N49" s="4" t="s">
         <v>9</v>
@@ -4996,7 +4996,7 @@
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>68</v>
@@ -5011,7 +5011,7 @@
         <v>9</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G50" s="4" t="s">
         <v>68</v>
@@ -5032,7 +5032,7 @@
         <v>333</v>
       </c>
       <c r="M50" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N50" s="4" t="s">
         <v>148</v>
@@ -5052,7 +5052,7 @@
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>68</v>
@@ -5067,7 +5067,7 @@
         <v>9</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G51" s="4" t="s">
         <v>68</v>
@@ -5088,7 +5088,7 @@
         <v>341</v>
       </c>
       <c r="M51" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N51" s="4" t="s">
         <v>9</v>
@@ -5108,7 +5108,7 @@
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>69</v>
@@ -5123,7 +5123,7 @@
         <v>56</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G52" s="4" t="s">
         <v>69</v>
@@ -5144,7 +5144,7 @@
         <v>331</v>
       </c>
       <c r="M52" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N52" s="4" t="s">
         <v>284</v>
@@ -5164,7 +5164,7 @@
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>69</v>
@@ -5179,7 +5179,7 @@
         <v>57</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G53" s="4" t="s">
         <v>69</v>
@@ -5200,7 +5200,7 @@
         <v>331</v>
       </c>
       <c r="M53" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N53" s="4" t="s">
         <v>284</v>
@@ -5220,7 +5220,7 @@
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>71</v>
@@ -5235,7 +5235,7 @@
         <v>73</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G54" s="4" t="s">
         <v>71</v>
@@ -5256,7 +5256,7 @@
         <v>331</v>
       </c>
       <c r="M54" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N54" s="4" t="s">
         <v>359</v>
@@ -5276,7 +5276,7 @@
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>71</v>
@@ -5291,7 +5291,7 @@
         <v>74</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G55" s="4" t="s">
         <v>71</v>
@@ -5312,7 +5312,7 @@
         <v>331</v>
       </c>
       <c r="M55" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N55" s="4" t="s">
         <v>359</v>
@@ -5332,7 +5332,7 @@
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>71</v>
@@ -5347,7 +5347,7 @@
         <v>75</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G56" s="4" t="s">
         <v>71</v>
@@ -5368,7 +5368,7 @@
         <v>331</v>
       </c>
       <c r="M56" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N56" s="4" t="s">
         <v>359</v>
@@ -5388,7 +5388,7 @@
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>71</v>
@@ -5403,7 +5403,7 @@
         <v>76</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G57" s="4" t="s">
         <v>71</v>
@@ -5424,7 +5424,7 @@
         <v>331</v>
       </c>
       <c r="M57" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N57" s="4" t="s">
         <v>359</v>
@@ -5444,7 +5444,7 @@
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>71</v>
@@ -5459,7 +5459,7 @@
         <v>73</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G58" s="4" t="s">
         <v>71</v>
@@ -5480,7 +5480,7 @@
         <v>331</v>
       </c>
       <c r="M58" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N58" s="4" t="s">
         <v>359</v>
@@ -5500,7 +5500,7 @@
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>71</v>
@@ -5515,7 +5515,7 @@
         <v>74</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G59" s="4" t="s">
         <v>71</v>
@@ -5536,7 +5536,7 @@
         <v>331</v>
       </c>
       <c r="M59" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N59" s="4" t="s">
         <v>359</v>
@@ -5556,7 +5556,7 @@
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>71</v>
@@ -5571,7 +5571,7 @@
         <v>75</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G60" s="4" t="s">
         <v>71</v>
@@ -5592,7 +5592,7 @@
         <v>331</v>
       </c>
       <c r="M60" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N60" s="4" t="s">
         <v>359</v>
@@ -5612,7 +5612,7 @@
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>71</v>
@@ -5627,7 +5627,7 @@
         <v>76</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G61" s="4" t="s">
         <v>71</v>
@@ -5648,7 +5648,7 @@
         <v>331</v>
       </c>
       <c r="M61" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N61" s="4" t="s">
         <v>359</v>
@@ -5668,7 +5668,7 @@
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B62" s="4" t="s">
         <v>77</v>
@@ -5683,7 +5683,7 @@
         <v>9</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G62" s="4" t="s">
         <v>77</v>
@@ -5704,7 +5704,7 @@
         <v>333</v>
       </c>
       <c r="M62" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N62" s="4" t="s">
         <v>284</v>
@@ -5724,7 +5724,7 @@
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B63" s="4" t="s">
         <v>77</v>
@@ -5739,7 +5739,7 @@
         <v>65</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G63" s="4" t="s">
         <v>77</v>
@@ -5760,7 +5760,7 @@
         <v>330</v>
       </c>
       <c r="M63" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N63" s="4" t="s">
         <v>284</v>
@@ -5780,7 +5780,7 @@
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B64" s="4" t="s">
         <v>77</v>
@@ -5795,7 +5795,7 @@
         <v>16</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G64" s="4" t="s">
         <v>77</v>
@@ -5816,7 +5816,7 @@
         <v>330</v>
       </c>
       <c r="M64" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N64" s="4" t="s">
         <v>284</v>
@@ -5836,7 +5836,7 @@
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B65" s="4" t="s">
         <v>77</v>
@@ -5851,7 +5851,7 @@
         <v>17</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G65" s="4" t="s">
         <v>77</v>
@@ -5872,7 +5872,7 @@
         <v>330</v>
       </c>
       <c r="M65" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N65" s="4" t="s">
         <v>284</v>
@@ -5892,7 +5892,7 @@
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B66" s="4" t="s">
         <v>79</v>
@@ -5907,7 +5907,7 @@
         <v>9</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G66" s="4" t="s">
         <v>79</v>
@@ -5928,7 +5928,7 @@
         <v>335</v>
       </c>
       <c r="M66" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N66" s="4" t="s">
         <v>285</v>
@@ -5948,7 +5948,7 @@
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B67" s="4" t="s">
         <v>80</v>
@@ -5963,7 +5963,7 @@
         <v>9</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G67" s="4" t="s">
         <v>80</v>
@@ -5984,7 +5984,7 @@
         <v>335</v>
       </c>
       <c r="M67" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N67" s="4" t="s">
         <v>285</v>
@@ -6004,7 +6004,7 @@
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B68" s="4" t="s">
         <v>80</v>
@@ -6019,7 +6019,7 @@
         <v>9</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G68" s="4" t="s">
         <v>80</v>
@@ -6040,7 +6040,7 @@
         <v>342</v>
       </c>
       <c r="M68" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N68" s="4" t="s">
         <v>9</v>
@@ -6060,7 +6060,7 @@
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B69" s="4" t="s">
         <v>82</v>
@@ -6075,7 +6075,7 @@
         <v>84</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G69" s="4" t="s">
         <v>82</v>
@@ -6096,7 +6096,7 @@
         <v>332</v>
       </c>
       <c r="M69" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N69" s="4" t="s">
         <v>284</v>
@@ -6116,7 +6116,7 @@
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B70" s="4" t="s">
         <v>82</v>
@@ -6131,7 +6131,7 @@
         <v>84</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G70" s="4" t="s">
         <v>82</v>
@@ -6152,7 +6152,7 @@
         <v>332</v>
       </c>
       <c r="M70" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N70" s="4" t="s">
         <v>284</v>
@@ -6172,7 +6172,7 @@
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B71" s="4" t="s">
         <v>85</v>
@@ -6187,7 +6187,7 @@
         <v>87</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G71" s="4" t="s">
         <v>85</v>
@@ -6208,7 +6208,7 @@
         <v>331</v>
       </c>
       <c r="M71" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N71" s="4" t="s">
         <v>359</v>
@@ -6228,7 +6228,7 @@
     </row>
     <row r="72" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B72" s="4" t="s">
         <v>85</v>
@@ -6243,7 +6243,7 @@
         <v>88</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G72" s="4" t="s">
         <v>85</v>
@@ -6264,7 +6264,7 @@
         <v>331</v>
       </c>
       <c r="M72" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N72" s="4" t="s">
         <v>359</v>
@@ -6284,7 +6284,7 @@
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B73" s="4" t="s">
         <v>85</v>
@@ -6299,7 +6299,7 @@
         <v>89</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G73" s="4" t="s">
         <v>85</v>
@@ -6320,7 +6320,7 @@
         <v>331</v>
       </c>
       <c r="M73" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N73" s="4" t="s">
         <v>359</v>
@@ -6340,7 +6340,7 @@
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B74" s="4" t="s">
         <v>85</v>
@@ -6355,7 +6355,7 @@
         <v>90</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G74" s="4" t="s">
         <v>85</v>
@@ -6376,7 +6376,7 @@
         <v>331</v>
       </c>
       <c r="M74" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N74" s="4" t="s">
         <v>359</v>
@@ -6396,7 +6396,7 @@
     </row>
     <row r="75" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B75" s="4" t="s">
         <v>91</v>
@@ -6411,7 +6411,7 @@
         <v>30</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G75" s="4" t="s">
         <v>91</v>
@@ -6432,7 +6432,7 @@
         <v>333</v>
       </c>
       <c r="M75" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N75" s="4" t="s">
         <v>135</v>
@@ -6452,7 +6452,7 @@
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B76" s="4" t="s">
         <v>91</v>
@@ -6467,7 +6467,7 @@
         <v>31</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G76" s="4" t="s">
         <v>91</v>
@@ -6488,7 +6488,7 @@
         <v>333</v>
       </c>
       <c r="M76" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N76" s="4" t="s">
         <v>135</v>
@@ -6508,7 +6508,7 @@
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B77" s="4" t="s">
         <v>91</v>
@@ -6523,7 +6523,7 @@
         <v>92</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G77" s="4" t="s">
         <v>91</v>
@@ -6544,7 +6544,7 @@
         <v>333</v>
       </c>
       <c r="M77" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N77" s="4" t="s">
         <v>135</v>

</xml_diff>

<commit_message>
Map20Tto21T add missing ley pop entries
</commit_message>
<xml_diff>
--- a/data-raw/snu_x_im_distribution_configuration/20Tto21TMap.xlsx
+++ b/data-raw/snu_x_im_distribution_configuration/20Tto21TMap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/snu_x_im_distribution_configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{F2764C82-AD4F-3848-8A79-A1E8798F0082}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{3160F7E5-1B0C-8445-A297-C85076E84FC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="19Tto20TMap" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Unused FY19 targets" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'19Tto20TMap'!$A$1:$N$87</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'19Tto20TMap'!$A$1:$N$91</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1582" uniqueCount="405">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1638" uniqueCount="409">
   <si>
     <t>indicatorCode</t>
   </si>
@@ -1254,6 +1254,18 @@
   </si>
   <si>
     <t>PMTCT PostANC/Age/Sex/Result</t>
+  </si>
+  <si>
+    <t>HTS_SELF.N.KeyPop.T</t>
+  </si>
+  <si>
+    <t>TX_CURR.N.KeyPop_HIVStatus.T</t>
+  </si>
+  <si>
+    <t>TX_PVLS.D.KeyPop_HIVStatus.T</t>
+  </si>
+  <si>
+    <t>TX_PVLS.N.KeyPop_HIVStatus.T</t>
   </si>
 </sst>
 </file>
@@ -1781,13 +1793,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2143,12 +2156,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N87"/>
+  <dimension ref="A1:N91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A44" sqref="A44"/>
-      <selection pane="topRight" activeCell="A6" sqref="A6"/>
+      <selection pane="topRight" activeCell="A80" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4019,8 +4032,8 @@
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
-        <v>402</v>
+      <c r="A43" s="6" t="s">
+        <v>405</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>361</v>
@@ -4056,51 +4069,51 @@
         <v>93</v>
       </c>
       <c r="M43" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N43" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="J44" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K44" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L44" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="M44" s="4" t="s">
         <v>223</v>
-      </c>
-      <c r="N43" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A44" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>361</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="G44" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H44" s="4" t="s">
-        <v>287</v>
-      </c>
-      <c r="I44" s="4" t="s">
-        <v>362</v>
-      </c>
-      <c r="J44" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K44" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="L44" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="M44" s="4" t="s">
-        <v>9</v>
       </c>
       <c r="N44" s="4" t="s">
         <v>92</v>
@@ -4108,16 +4121,16 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>361</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>52</v>
@@ -4126,10 +4139,10 @@
         <v>247</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>279</v>
+        <v>287</v>
       </c>
       <c r="I45" s="4" t="s">
         <v>362</v>
@@ -4138,10 +4151,10 @@
         <v>9</v>
       </c>
       <c r="K45" s="4" t="s">
-        <v>9</v>
+        <v>88</v>
       </c>
       <c r="L45" s="4" t="s">
-        <v>224</v>
+        <v>9</v>
       </c>
       <c r="M45" s="4" t="s">
         <v>9</v>
@@ -4152,16 +4165,16 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>361</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>52</v>
@@ -4170,10 +4183,10 @@
         <v>247</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>59</v>
+        <v>25</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="I46" s="4" t="s">
         <v>362</v>
@@ -4185,7 +4198,7 @@
         <v>9</v>
       </c>
       <c r="L46" s="4" t="s">
-        <v>9</v>
+        <v>224</v>
       </c>
       <c r="M46" s="4" t="s">
         <v>9</v>
@@ -4196,16 +4209,16 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>332</v>
+        <v>299</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>361</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>52</v>
@@ -4214,25 +4227,25 @@
         <v>247</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
       <c r="I47" s="4" t="s">
         <v>362</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>225</v>
+        <v>9</v>
       </c>
       <c r="K47" s="4" t="s">
-        <v>88</v>
+        <v>9</v>
       </c>
       <c r="L47" s="4" t="s">
         <v>9</v>
       </c>
       <c r="M47" s="4" t="s">
-        <v>367</v>
+        <v>9</v>
       </c>
       <c r="N47" s="4" t="s">
         <v>92</v>
@@ -4240,7 +4253,7 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>361</v>
@@ -4276,7 +4289,7 @@
         <v>9</v>
       </c>
       <c r="M48" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="N48" s="4" t="s">
         <v>92</v>
@@ -4284,16 +4297,16 @@
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>361</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>52</v>
@@ -4302,25 +4315,25 @@
         <v>247</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>369</v>
+        <v>32</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>370</v>
+        <v>271</v>
       </c>
       <c r="I49" s="4" t="s">
         <v>362</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>87</v>
+        <v>225</v>
       </c>
       <c r="K49" s="4" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="L49" s="4" t="s">
         <v>9</v>
       </c>
       <c r="M49" s="4" t="s">
-        <v>226</v>
+        <v>368</v>
       </c>
       <c r="N49" s="4" t="s">
         <v>92</v>
@@ -4328,7 +4341,7 @@
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>361</v>
@@ -4364,7 +4377,7 @@
         <v>9</v>
       </c>
       <c r="M50" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="N50" s="4" t="s">
         <v>92</v>
@@ -4372,16 +4385,16 @@
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
-        <v>300</v>
+        <v>335</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>361</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>52</v>
@@ -4390,25 +4403,25 @@
         <v>247</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>30</v>
+        <v>369</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>269</v>
+        <v>370</v>
       </c>
       <c r="I51" s="4" t="s">
         <v>362</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="K51" s="4" t="s">
-        <v>9</v>
+        <v>97</v>
       </c>
       <c r="L51" s="4" t="s">
         <v>9</v>
       </c>
       <c r="M51" s="4" t="s">
-        <v>9</v>
+        <v>227</v>
       </c>
       <c r="N51" s="4" t="s">
         <v>92</v>
@@ -4416,7 +4429,7 @@
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>361</v>
@@ -4443,7 +4456,7 @@
         <v>362</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K52" s="4" t="s">
         <v>9</v>
@@ -4460,37 +4473,37 @@
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>336</v>
+        <v>301</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>361</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I53" s="4" t="s">
         <v>362</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="K53" s="4" t="s">
-        <v>97</v>
+        <v>9</v>
       </c>
       <c r="L53" s="4" t="s">
         <v>9</v>
@@ -4504,7 +4517,7 @@
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>361</v>
@@ -4516,16 +4529,16 @@
         <v>257</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="I54" s="4" t="s">
         <v>362</v>
@@ -4540,7 +4553,7 @@
         <v>9</v>
       </c>
       <c r="M54" s="4" t="s">
-        <v>228</v>
+        <v>9</v>
       </c>
       <c r="N54" s="4" t="s">
         <v>92</v>
@@ -4548,7 +4561,7 @@
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>361</v>
@@ -4584,7 +4597,7 @@
         <v>9</v>
       </c>
       <c r="M55" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="N55" s="4" t="s">
         <v>92</v>
@@ -4592,7 +4605,7 @@
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>361</v>
@@ -4628,15 +4641,15 @@
         <v>9</v>
       </c>
       <c r="M56" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="N56" s="4" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
-        <v>393</v>
+      <c r="A57" s="4" t="s">
+        <v>339</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>361</v>
@@ -4663,7 +4676,7 @@
         <v>362</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="K57" s="4" t="s">
         <v>97</v>
@@ -4679,17 +4692,17 @@
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A58" s="4" t="s">
-        <v>340</v>
+      <c r="A58" s="1" t="s">
+        <v>393</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>361</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E58" s="4" t="s">
         <v>52</v>
@@ -4698,25 +4711,25 @@
         <v>247</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="I58" s="4" t="s">
         <v>362</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K58" s="4" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="L58" s="4" t="s">
         <v>9</v>
       </c>
       <c r="M58" s="4" t="s">
-        <v>9</v>
+        <v>230</v>
       </c>
       <c r="N58" s="4" t="s">
         <v>92</v>
@@ -4724,16 +4737,16 @@
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>361</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>376</v>
+        <v>258</v>
       </c>
       <c r="E59" s="4" t="s">
         <v>52</v>
@@ -4751,7 +4764,7 @@
         <v>362</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="K59" s="4" t="s">
         <v>88</v>
@@ -4768,7 +4781,7 @@
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
-        <v>302</v>
+        <v>341</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>361</v>
@@ -4786,22 +4799,22 @@
         <v>247</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="H60" s="4" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="I60" s="4" t="s">
         <v>362</v>
       </c>
       <c r="J60" s="4" t="s">
-        <v>9</v>
+        <v>98</v>
       </c>
       <c r="K60" s="4" t="s">
-        <v>9</v>
+        <v>88</v>
       </c>
       <c r="L60" s="4" t="s">
-        <v>93</v>
+        <v>9</v>
       </c>
       <c r="M60" s="4" t="s">
         <v>9</v>
@@ -4812,16 +4825,16 @@
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
-        <v>342</v>
+        <v>302</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>361</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>259</v>
+        <v>376</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>52</v>
@@ -4830,22 +4843,22 @@
         <v>247</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="H61" s="4" t="s">
-        <v>271</v>
+        <v>279</v>
       </c>
       <c r="I61" s="4" t="s">
         <v>362</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>98</v>
+        <v>9</v>
       </c>
       <c r="K61" s="4" t="s">
-        <v>88</v>
+        <v>9</v>
       </c>
       <c r="L61" s="4" t="s">
-        <v>9</v>
+        <v>93</v>
       </c>
       <c r="M61" s="4" t="s">
         <v>9</v>
@@ -4856,7 +4869,7 @@
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
-        <v>303</v>
+        <v>342</v>
       </c>
       <c r="B62" s="4" t="s">
         <v>361</v>
@@ -4874,22 +4887,22 @@
         <v>247</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="I62" s="4" t="s">
         <v>362</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>9</v>
+        <v>98</v>
       </c>
       <c r="K62" s="4" t="s">
-        <v>9</v>
+        <v>88</v>
       </c>
       <c r="L62" s="4" t="s">
-        <v>93</v>
+        <v>9</v>
       </c>
       <c r="M62" s="4" t="s">
         <v>9</v>
@@ -4900,16 +4913,16 @@
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
-        <v>343</v>
+        <v>303</v>
       </c>
       <c r="B63" s="4" t="s">
         <v>361</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E63" s="4" t="s">
         <v>52</v>
@@ -4918,22 +4931,22 @@
         <v>247</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>270</v>
+        <v>279</v>
       </c>
       <c r="I63" s="4" t="s">
         <v>362</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>231</v>
+        <v>9</v>
       </c>
       <c r="K63" s="4" t="s">
-        <v>88</v>
+        <v>9</v>
       </c>
       <c r="L63" s="4" t="s">
-        <v>9</v>
+        <v>93</v>
       </c>
       <c r="M63" s="4" t="s">
         <v>9</v>
@@ -4944,7 +4957,7 @@
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B64" s="4" t="s">
         <v>361</v>
@@ -4988,34 +5001,34 @@
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
-        <v>373</v>
+        <v>344</v>
       </c>
       <c r="B65" s="4" t="s">
         <v>361</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="H65" s="4" t="s">
-        <v>371</v>
+        <v>270</v>
       </c>
       <c r="I65" s="4" t="s">
         <v>362</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>295</v>
+        <v>231</v>
       </c>
       <c r="K65" s="4" t="s">
         <v>88</v>
@@ -5024,7 +5037,7 @@
         <v>9</v>
       </c>
       <c r="M65" s="4" t="s">
-        <v>226</v>
+        <v>9</v>
       </c>
       <c r="N65" s="4" t="s">
         <v>92</v>
@@ -5032,7 +5045,7 @@
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B66" s="4" t="s">
         <v>361</v>
@@ -5068,7 +5081,7 @@
         <v>9</v>
       </c>
       <c r="M66" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="N66" s="4" t="s">
         <v>92</v>
@@ -5076,7 +5089,7 @@
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="B67" s="4" t="s">
         <v>361</v>
@@ -5088,10 +5101,10 @@
         <v>261</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="G67" s="4" t="s">
         <v>39</v>
@@ -5112,7 +5125,7 @@
         <v>9</v>
       </c>
       <c r="M67" s="4" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="N67" s="4" t="s">
         <v>92</v>
@@ -5120,7 +5133,7 @@
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B68" s="4" t="s">
         <v>361</v>
@@ -5156,7 +5169,7 @@
         <v>9</v>
       </c>
       <c r="M68" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="N68" s="4" t="s">
         <v>92</v>
@@ -5164,34 +5177,34 @@
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
-        <v>345</v>
+        <v>374</v>
       </c>
       <c r="B69" s="4" t="s">
         <v>361</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G69" s="4" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="H69" s="4" t="s">
-        <v>271</v>
+        <v>371</v>
       </c>
       <c r="I69" s="4" t="s">
         <v>362</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>231</v>
+        <v>295</v>
       </c>
       <c r="K69" s="4" t="s">
         <v>88</v>
@@ -5200,7 +5213,7 @@
         <v>9</v>
       </c>
       <c r="M69" s="4" t="s">
-        <v>9</v>
+        <v>227</v>
       </c>
       <c r="N69" s="4" t="s">
         <v>92</v>
@@ -5208,7 +5221,7 @@
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B70" s="4" t="s">
         <v>361</v>
@@ -5220,16 +5233,16 @@
         <v>262</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H70" s="4" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="I70" s="4" t="s">
         <v>362</v>
@@ -5244,7 +5257,7 @@
         <v>9</v>
       </c>
       <c r="M70" s="4" t="s">
-        <v>228</v>
+        <v>9</v>
       </c>
       <c r="N70" s="4" t="s">
         <v>92</v>
@@ -5252,7 +5265,7 @@
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B71" s="4" t="s">
         <v>361</v>
@@ -5288,7 +5301,7 @@
         <v>9</v>
       </c>
       <c r="M71" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="N71" s="4" t="s">
         <v>92</v>
@@ -5296,7 +5309,7 @@
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B72" s="4" t="s">
         <v>361</v>
@@ -5332,15 +5345,15 @@
         <v>9</v>
       </c>
       <c r="M72" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="N72" s="4" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A73" s="1" t="s">
-        <v>392</v>
+      <c r="A73" s="4" t="s">
+        <v>348</v>
       </c>
       <c r="B73" s="4" t="s">
         <v>361</v>
@@ -5367,7 +5380,7 @@
         <v>362</v>
       </c>
       <c r="J73" s="4" t="s">
-        <v>98</v>
+        <v>231</v>
       </c>
       <c r="K73" s="4" t="s">
         <v>88</v>
@@ -5383,17 +5396,17 @@
       </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A74" s="4" t="s">
-        <v>349</v>
+      <c r="A74" s="1" t="s">
+        <v>392</v>
       </c>
       <c r="B74" s="4" t="s">
         <v>361</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E74" s="4" t="s">
         <v>52</v>
@@ -5402,16 +5415,16 @@
         <v>247</v>
       </c>
       <c r="G74" s="4" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="H74" s="4" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="I74" s="4" t="s">
         <v>362</v>
       </c>
       <c r="J74" s="4" t="s">
-        <v>231</v>
+        <v>98</v>
       </c>
       <c r="K74" s="4" t="s">
         <v>88</v>
@@ -5420,7 +5433,7 @@
         <v>9</v>
       </c>
       <c r="M74" s="4" t="s">
-        <v>9</v>
+        <v>230</v>
       </c>
       <c r="N74" s="4" t="s">
         <v>92</v>
@@ -5428,16 +5441,16 @@
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B75" s="4" t="s">
         <v>361</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E75" s="4" t="s">
         <v>52</v>
@@ -5472,7 +5485,7 @@
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B76" s="4" t="s">
         <v>361</v>
@@ -5490,22 +5503,22 @@
         <v>247</v>
       </c>
       <c r="G76" s="4" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="H76" s="4" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="I76" s="4" t="s">
         <v>362</v>
       </c>
       <c r="J76" s="4" t="s">
-        <v>9</v>
+        <v>231</v>
       </c>
       <c r="K76" s="4" t="s">
-        <v>9</v>
+        <v>88</v>
       </c>
       <c r="L76" s="4" t="s">
-        <v>93</v>
+        <v>9</v>
       </c>
       <c r="M76" s="4" t="s">
         <v>9</v>
@@ -5516,43 +5529,43 @@
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B77" s="4" t="s">
         <v>361</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G77" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H77" s="4" t="s">
-        <v>377</v>
+        <v>280</v>
       </c>
       <c r="I77" s="4" t="s">
         <v>362</v>
       </c>
       <c r="J77" s="4" t="s">
-        <v>231</v>
+        <v>9</v>
       </c>
       <c r="K77" s="4" t="s">
-        <v>88</v>
+        <v>9</v>
       </c>
       <c r="L77" s="4" t="s">
-        <v>9</v>
+        <v>93</v>
       </c>
       <c r="M77" s="4" t="s">
-        <v>240</v>
+        <v>9</v>
       </c>
       <c r="N77" s="4" t="s">
         <v>92</v>
@@ -5560,43 +5573,43 @@
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
-        <v>353</v>
+        <v>406</v>
       </c>
       <c r="B78" s="4" t="s">
         <v>361</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G78" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H78" s="4" t="s">
-        <v>377</v>
+        <v>280</v>
       </c>
       <c r="I78" s="4" t="s">
         <v>362</v>
       </c>
       <c r="J78" s="4" t="s">
-        <v>231</v>
+        <v>9</v>
       </c>
       <c r="K78" s="4" t="s">
-        <v>88</v>
+        <v>9</v>
       </c>
       <c r="L78" s="4" t="s">
-        <v>9</v>
+        <v>93</v>
       </c>
       <c r="M78" s="4" t="s">
-        <v>240</v>
+        <v>9</v>
       </c>
       <c r="N78" s="4" t="s">
         <v>92</v>
@@ -5604,43 +5617,43 @@
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
-        <v>354</v>
+        <v>407</v>
       </c>
       <c r="B79" s="4" t="s">
         <v>361</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G79" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="H79" s="4" t="s">
-        <v>381</v>
+        <v>280</v>
       </c>
       <c r="I79" s="4" t="s">
         <v>362</v>
       </c>
       <c r="J79" s="4" t="s">
-        <v>295</v>
+        <v>9</v>
       </c>
       <c r="K79" s="4" t="s">
-        <v>88</v>
+        <v>9</v>
       </c>
       <c r="L79" s="4" t="s">
-        <v>9</v>
+        <v>93</v>
       </c>
       <c r="M79" s="4" t="s">
-        <v>382</v>
+        <v>9</v>
       </c>
       <c r="N79" s="4" t="s">
         <v>92</v>
@@ -5648,43 +5661,43 @@
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
-        <v>355</v>
+        <v>408</v>
       </c>
       <c r="B80" s="4" t="s">
         <v>361</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G80" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="H80" s="4" t="s">
-        <v>381</v>
+        <v>280</v>
       </c>
       <c r="I80" s="4" t="s">
         <v>362</v>
       </c>
       <c r="J80" s="4" t="s">
-        <v>295</v>
+        <v>9</v>
       </c>
       <c r="K80" s="4" t="s">
-        <v>88</v>
+        <v>9</v>
       </c>
       <c r="L80" s="4" t="s">
-        <v>9</v>
+        <v>93</v>
       </c>
       <c r="M80" s="4" t="s">
-        <v>383</v>
+        <v>9</v>
       </c>
       <c r="N80" s="4" t="s">
         <v>92</v>
@@ -5692,16 +5705,16 @@
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="B81" s="4" t="s">
         <v>361</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E81" s="4" t="s">
         <v>50</v>
@@ -5710,16 +5723,16 @@
         <v>248</v>
       </c>
       <c r="G81" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H81" s="4" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="I81" s="4" t="s">
         <v>362</v>
       </c>
       <c r="J81" s="4" t="s">
-        <v>295</v>
+        <v>231</v>
       </c>
       <c r="K81" s="4" t="s">
         <v>88</v>
@@ -5728,7 +5741,7 @@
         <v>9</v>
       </c>
       <c r="M81" s="4" t="s">
-        <v>384</v>
+        <v>240</v>
       </c>
       <c r="N81" s="4" t="s">
         <v>92</v>
@@ -5736,16 +5749,16 @@
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="B82" s="4" t="s">
         <v>361</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E82" s="4" t="s">
         <v>50</v>
@@ -5754,16 +5767,16 @@
         <v>248</v>
       </c>
       <c r="G82" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H82" s="4" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="I82" s="4" t="s">
         <v>362</v>
       </c>
       <c r="J82" s="4" t="s">
-        <v>295</v>
+        <v>231</v>
       </c>
       <c r="K82" s="4" t="s">
         <v>88</v>
@@ -5772,7 +5785,7 @@
         <v>9</v>
       </c>
       <c r="M82" s="4" t="s">
-        <v>385</v>
+        <v>240</v>
       </c>
       <c r="N82" s="4" t="s">
         <v>92</v>
@@ -5780,43 +5793,43 @@
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="B83" s="4" t="s">
         <v>361</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="G83" s="4" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="H83" s="4" t="s">
-        <v>273</v>
+        <v>381</v>
       </c>
       <c r="I83" s="4" t="s">
         <v>362</v>
       </c>
       <c r="J83" s="4" t="s">
-        <v>98</v>
+        <v>295</v>
       </c>
       <c r="K83" s="4" t="s">
-        <v>241</v>
+        <v>88</v>
       </c>
       <c r="L83" s="4" t="s">
         <v>9</v>
       </c>
       <c r="M83" s="4" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="N83" s="4" t="s">
         <v>92</v>
@@ -5824,87 +5837,87 @@
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B84" s="4" t="s">
         <v>361</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="G84" s="4" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="H84" s="4" t="s">
-        <v>273</v>
+        <v>381</v>
       </c>
       <c r="I84" s="4" t="s">
         <v>362</v>
       </c>
       <c r="J84" s="4" t="s">
-        <v>98</v>
+        <v>295</v>
       </c>
       <c r="K84" s="4" t="s">
-        <v>241</v>
+        <v>88</v>
       </c>
       <c r="L84" s="4" t="s">
         <v>9</v>
       </c>
       <c r="M84" s="4" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
       <c r="N84" s="4" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A85" s="1" t="s">
-        <v>395</v>
+      <c r="A85" s="4" t="s">
+        <v>356</v>
       </c>
       <c r="B85" s="4" t="s">
         <v>361</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E85" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="G85" s="4" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="H85" s="4" t="s">
-        <v>273</v>
+        <v>381</v>
       </c>
       <c r="I85" s="4" t="s">
         <v>362</v>
       </c>
       <c r="J85" s="4" t="s">
-        <v>98</v>
+        <v>295</v>
       </c>
       <c r="K85" s="4" t="s">
-        <v>241</v>
+        <v>88</v>
       </c>
       <c r="L85" s="4" t="s">
         <v>9</v>
       </c>
       <c r="M85" s="4" t="s">
-        <v>379</v>
+        <v>384</v>
       </c>
       <c r="N85" s="4" t="s">
         <v>92</v>
@@ -5912,43 +5925,43 @@
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="B86" s="4" t="s">
         <v>361</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E86" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F86" s="4" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="G86" s="4" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="H86" s="4" t="s">
-        <v>273</v>
+        <v>381</v>
       </c>
       <c r="I86" s="4" t="s">
         <v>362</v>
       </c>
       <c r="J86" s="4" t="s">
-        <v>98</v>
+        <v>295</v>
       </c>
       <c r="K86" s="4" t="s">
-        <v>241</v>
+        <v>88</v>
       </c>
       <c r="L86" s="4" t="s">
         <v>9</v>
       </c>
       <c r="M86" s="4" t="s">
-        <v>380</v>
+        <v>385</v>
       </c>
       <c r="N86" s="4" t="s">
         <v>92</v>
@@ -5956,16 +5969,16 @@
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
-        <v>386</v>
+        <v>358</v>
       </c>
       <c r="B87" s="4" t="s">
         <v>361</v>
       </c>
-      <c r="C87" s="5" t="s">
-        <v>6</v>
+      <c r="C87" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>387</v>
+        <v>267</v>
       </c>
       <c r="E87" s="4" t="s">
         <v>52</v>
@@ -5982,26 +5995,202 @@
       <c r="I87" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="J87" s="5" t="s">
+      <c r="J87" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="K87" s="5" t="s">
+      <c r="K87" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="L87" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M87" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="N87" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A88" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D88" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F88" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="G88" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H88" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="I88" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="J88" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="K88" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="L88" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M88" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="N88" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D89" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="E89" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F89" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="G89" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H89" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="I89" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="J89" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="K89" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="L89" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M89" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="N89" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A90" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D90" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="E90" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F90" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="G90" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H90" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="I90" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="J90" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="K90" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="L90" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M90" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="N90" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A91" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D91" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="E91" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F91" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="G91" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H91" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="I91" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="J91" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="K91" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="L87" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="M87" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="N87" s="5" t="s">
+      <c r="L91" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M91" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="N91" s="5" t="s">
         <v>92</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N87" xr:uid="{1831349A-3542-5B45-8A69-A97FE54E5E29}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N87">
-    <sortCondition ref="A2:A87"/>
+  <autoFilter ref="A1:N91" xr:uid="{1831349A-3542-5B45-8A69-A97FE54E5E29}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N91">
+    <sortCondition ref="A2:A91"/>
   </sortState>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Map20Tto21T fix config error for OVC_SERV
</commit_message>
<xml_diff>
--- a/data-raw/snu_x_im_distribution_configuration/20Tto21TMap.xlsx
+++ b/data-raw/snu_x_im_distribution_configuration/20Tto21TMap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/snu_x_im_distribution_configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{3160F7E5-1B0C-8445-A297-C85076E84FC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D95ECAC2-7187-894E-826F-0FBF05B610F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1638" uniqueCount="409">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1638" uniqueCount="411">
   <si>
     <t>indicatorCode</t>
   </si>
@@ -1266,13 +1266,19 @@
   </si>
   <si>
     <t>TX_PVLS.N.KeyPop_HIVStatus.T</t>
+  </si>
+  <si>
+    <t>Age/Sex/ProgramStatus</t>
+  </si>
+  <si>
+    <t>QG5SE83IVmL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1418,6 +1424,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC5C8C6"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="34">
@@ -1793,7 +1805,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -1801,6 +1813,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2158,10 +2171,10 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A44" sqref="A44"/>
-      <selection pane="topRight" activeCell="A80" sqref="A80"/>
+      <selection pane="topRight" activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4270,11 +4283,11 @@
       <c r="F48" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="G48" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H48" s="4" t="s">
-        <v>271</v>
+      <c r="G48" s="7" t="s">
+        <v>409</v>
+      </c>
+      <c r="H48" s="7" t="s">
+        <v>410</v>
       </c>
       <c r="I48" s="4" t="s">
         <v>362</v>
@@ -4314,11 +4327,11 @@
       <c r="F49" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="G49" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H49" s="4" t="s">
-        <v>271</v>
+      <c r="G49" s="7" t="s">
+        <v>409</v>
+      </c>
+      <c r="H49" s="7" t="s">
+        <v>410</v>
       </c>
       <c r="I49" s="4" t="s">
         <v>362</v>

</xml_diff>

<commit_message>
SNUxIM distribution ready for full run of all countries
</commit_message>
<xml_diff>
--- a/data-raw/snu_x_im_distribution_configuration/20Tto21TMap.xlsx
+++ b/data-raw/snu_x_im_distribution_configuration/20Tto21TMap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/snu_x_im_distribution_configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D95ECAC2-7187-894E-826F-0FBF05B610F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{4DD38D8A-2EFB-844F-9D1B-208FD34B1B9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1813,7 +1813,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2171,10 +2171,10 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A44" sqref="A44"/>
-      <selection pane="topRight" activeCell="G46" sqref="G46"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>